<commit_message>
Implemented ZipBreakerAkka2 - less Akka features used, but simpler and highly efficient design.
</commit_message>
<xml_diff>
--- a/ZipBreakerAkka/src/main/resources/PerformanceTests.xlsx
+++ b/ZipBreakerAkka/src/main/resources/PerformanceTests.xlsx
@@ -814,11 +814,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="104744448"/>
-        <c:axId val="92694784"/>
+        <c:axId val="90804736"/>
+        <c:axId val="50504832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="104744448"/>
+        <c:axId val="90804736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -827,7 +827,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92694784"/>
+        <c:crossAx val="50504832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -835,7 +835,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92694784"/>
+        <c:axId val="50504832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -846,7 +846,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104744448"/>
+        <c:crossAx val="90804736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -858,6 +858,175 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Processing Time Comparison </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>(1 million passwords)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Processing Time Comparison (1 million passwords)</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$3:$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Classic Java code
+(single threaded)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Java - Fork Join
+(single JVM)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Akka Distributed
+(single physical machine)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>672857</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>307537</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18983552</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="90806272"/>
+        <c:axId val="50507136"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="90806272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50507136"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50507136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90806272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
@@ -895,6 +1064,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1285874</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>195262</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>542924</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1193,7 +1392,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>